<commit_message>
Script Update for new Game Mechanic
Berechnung ist jetzt darauf ausgelegt, dass die Bonusperson in Gruppe 11 nicht mehr bekannt sein muss.
Klassische Berechnung inklusive Optimierung unverändert.
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
     <sheet name="Matchboxen" sheetId="2" r:id="rId2"/>
     <sheet name="MatchingNights" sheetId="3" r:id="rId3"/>
+    <sheet name="Sonstiges" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -101,18 +102,12 @@
     <t>nein</t>
   </si>
   <si>
-    <t>Hier die Ergebnisse der bis zu 10 Matchboxen eintragen.</t>
-  </si>
-  <si>
     <t>Matches</t>
   </si>
   <si>
     <t>MatchingNights</t>
   </si>
   <si>
-    <t>Bei Matches zwischen Paaren daran denken, die entsprechenden NoMatches mit der Extra-Person einzutragen.</t>
-  </si>
-  <si>
     <t>Nur orangene Felder beschreiben (grün wenn befüllt). Die größere Gruppe ist die, zu der später noch ein/e NachzüglerIn kommt</t>
   </si>
   <si>
@@ -122,9 +117,60 @@
     <t>Hier die Paarungen und Anzahl der korrekten Matches der bis zu 10 MatchingNights eintragen. Zeile komplett befüllen oder komplett leer lassen. Fallen Nächte aus, die vorherige Nacht 1zu1 kopieren</t>
   </si>
   <si>
+    <t>Passwort zum Entsperren der Seiten: "ayto" (nicht empfohlen!)</t>
+  </si>
+  <si>
     <t>optional Anmerkungen (nicht ausgewertet)</t>
   </si>
   <si>
+    <t>Uniqe</t>
+  </si>
+  <si>
+    <t>In Spalte Unique angeben, ob beide MatchpartnerInnen nur dieses (einzigartige) Match haben. Dann werden NoMatches automatisch für den Rest übernommen</t>
+  </si>
+  <si>
+    <t>Falls ein Doppelmatch gefunden wird, muss Unique auf nein gesetzt werden und alle weiteren NoMatches müssen manuell ergänzt werden.</t>
+  </si>
+  <si>
+    <t>Person 11 ist zusätzliches Match</t>
+  </si>
+  <si>
+    <t>Falls NachzüglerIn als zusätzliches Match bekannt ist, unbedingt bei ID 11 eintragen und Kästchen auf "ja" setzen</t>
+  </si>
+  <si>
+    <t>Barkin</t>
+  </si>
+  <si>
+    <t>Burim</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Deniz</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Kenneth</t>
+  </si>
+  <si>
+    <t>Maximilian</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Sasa</t>
+  </si>
+  <si>
+    <t>Marwin</t>
+  </si>
+  <si>
     <t>Aurelia</t>
   </si>
   <si>
@@ -149,43 +195,28 @@
     <t>Stefanie</t>
   </si>
   <si>
-    <t>Valerie</t>
-  </si>
-  <si>
     <t>Vanessa</t>
   </si>
   <si>
-    <t>Barkin</t>
-  </si>
-  <si>
-    <t>Burim</t>
-  </si>
-  <si>
-    <t>Christopher</t>
-  </si>
-  <si>
-    <t>Deniz</t>
-  </si>
-  <si>
-    <t>Joel</t>
-  </si>
-  <si>
-    <t>Ken</t>
-  </si>
-  <si>
-    <t>Kenneth</t>
-  </si>
-  <si>
-    <t>Maximilian</t>
-  </si>
-  <si>
-    <t>Pascal</t>
-  </si>
-  <si>
-    <t>Sasa</t>
-  </si>
-  <si>
-    <t>Marwin</t>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Box 1, Folge 1</t>
+  </si>
+  <si>
+    <t>Box 5, Folge 8 - 9</t>
+  </si>
+  <si>
+    <t>Box 4, Folge 6 - 7</t>
+  </si>
+  <si>
+    <t>Box 3, Folge 4 - 5</t>
+  </si>
+  <si>
+    <t>Box 2, Folge 2 - 3</t>
+  </si>
+  <si>
+    <t>Hier die Ergebnisse der bis zu 10 Matchboxen eintragen. Spalte KandidatInA&amp;B sowie Match sind Pflicht, Unique optional für Auswertung (nur bei Match relevant)</t>
   </si>
 </sst>
 </file>
@@ -428,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,6 +521,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -521,7 +558,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -540,6 +577,34 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -861,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,13 +962,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -911,13 +976,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -925,13 +990,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -939,13 +1004,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -953,13 +1018,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -967,13 +1032,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -981,13 +1046,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -995,13 +1060,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -1009,13 +1074,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1023,13 +1088,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -1037,41 +1102,87 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="F3:F13" name="Gruppe B"/>
-    <protectedRange sqref="C3:C12" name="Gruppe A"/>
+    <protectedRange sqref="E15" name="Bonusperson"/>
+    <protectedRange sqref="C3:C12" name="Gruppe A_1"/>
+    <protectedRange sqref="F3:F13" name="Gruppe B_1"/>
   </protectedRanges>
-  <mergeCells count="2">
-    <mergeCell ref="B15:H15"/>
+  <mergeCells count="3">
+    <mergeCell ref="B17:H17"/>
     <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B18:H18"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F13 C3:C12">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F13">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C12">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15">
+      <formula1>$B$20:$B$21</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1079,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AB26"/>
+  <dimension ref="B1:AD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,27 +1203,31 @@
     <col min="3" max="4" width="15.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
     <col min="6" max="6" width="1.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" style="3" customWidth="1"/>
-    <col min="8" max="27" width="9.140625" style="3"/>
-    <col min="28" max="28" width="0" style="3" hidden="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="8" style="3" customWidth="1"/>
+    <col min="8" max="8" width="1.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" style="3" customWidth="1"/>
+    <col min="10" max="29" width="9.140625" style="3"/>
+    <col min="30" max="30" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+    <row r="1" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="AB2" s="8" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="AD2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1126,264 +1241,376 @@
         <v>9</v>
       </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7"/>
-      <c r="AB4" s="5" t="s">
+      <c r="C4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F4" s="30"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>5</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="28"/>
-    </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F8" s="30"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>6</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F9" s="30"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>7</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F10" s="30"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>8</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F11" s="30"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>9</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F12" s="30"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>10</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F13" s="30"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>11</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F14" s="30"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>12</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="F15" s="30"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>13</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F16" s="30"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>14</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="30"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>15</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="30"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>16</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="30"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>17</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="30"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>18</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="30"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>19</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="30"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>20</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="C4:G23" name="Eingabe"/>
+    <protectedRange sqref="C4:I23" name="Eingabe_3"/>
   </protectedRanges>
-  <mergeCells count="3">
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B2:G2"/>
+  <mergeCells count="4">
+    <mergeCell ref="B25:N25"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B27:N27"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:F23">
+  <conditionalFormatting sqref="C4:H7 C9:H10 C12:H23">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:H8">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:H11">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:F23">
-      <formula1>$AB$3:$AB$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G23 E4:E23">
+      <formula1>$AD$3:$AD$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1392,15 +1619,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>TeilnehmerInnen!$F$3:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>TeilnehmerInnen!$C$3:$C$12</xm:f>
           </x14:formula1>
           <xm:sqref>C4:C23</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>TeilnehmerInnen!$F$3:$F$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4:D23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1412,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57:D58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,23 +1657,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="37"/>
+      <c r="B2" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1486,7 +1713,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="33">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
@@ -1523,7 +1750,7 @@
       </c>
       <c r="L5" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M5" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -1531,26 +1758,48 @@
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P5" s="21"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="N6" s="13"/>
-      <c r="O6" s="27"/>
+      <c r="O6" s="27">
+        <v>3</v>
+      </c>
       <c r="P6" s="21"/>
     </row>
     <row r="7" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1609,7 +1858,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="33">
+      <c r="C10" s="35">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
@@ -1646,7 +1895,7 @@
       </c>
       <c r="L10" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M10" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -1654,26 +1903,48 @@
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P10" s="21"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="N11" s="13"/>
-      <c r="O11" s="27"/>
+      <c r="O11" s="27">
+        <v>3</v>
+      </c>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1732,7 +2003,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="33">
+      <c r="C15" s="35">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
@@ -1769,7 +2040,7 @@
       </c>
       <c r="L15" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M15" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -1777,26 +2048,48 @@
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P15" s="21"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="N16" s="13"/>
-      <c r="O16" s="27"/>
+      <c r="O16" s="27">
+        <v>2</v>
+      </c>
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1855,7 +2148,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="33">
+      <c r="C20" s="35">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
@@ -1892,7 +2185,7 @@
       </c>
       <c r="L20" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M20" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -1900,14 +2193,14 @@
       </c>
       <c r="N20" s="13"/>
       <c r="O20" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P20" s="21"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="34"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
@@ -1978,7 +2271,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="33">
+      <c r="C25" s="35">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
@@ -2015,7 +2308,7 @@
       </c>
       <c r="L25" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M25" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2023,14 +2316,14 @@
       </c>
       <c r="N25" s="13"/>
       <c r="O25" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P25" s="21"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="34"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2101,7 +2394,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="33">
+      <c r="C30" s="35">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
@@ -2138,7 +2431,7 @@
       </c>
       <c r="L30" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M30" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2146,14 +2439,14 @@
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P30" s="21"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="34"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2224,7 +2517,7 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="33">
+      <c r="C35" s="35">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
@@ -2261,7 +2554,7 @@
       </c>
       <c r="L35" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M35" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2269,14 +2562,14 @@
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P35" s="21"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="34"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2347,7 +2640,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="33">
+      <c r="C40" s="35">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
@@ -2384,7 +2677,7 @@
       </c>
       <c r="L40" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M40" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2392,14 +2685,14 @@
       </c>
       <c r="N40" s="13"/>
       <c r="O40" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P40" s="21"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="34"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2470,7 +2763,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="33">
+      <c r="C45" s="35">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -2507,7 +2800,7 @@
       </c>
       <c r="L45" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M45" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2515,14 +2808,14 @@
       </c>
       <c r="N45" s="13"/>
       <c r="O45" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P45" s="21"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="34"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2593,7 +2886,7 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="33">
+      <c r="C50" s="35">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
@@ -2630,7 +2923,7 @@
       </c>
       <c r="L50" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valerie</v>
+        <v>Valeria</v>
       </c>
       <c r="M50" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
@@ -2638,14 +2931,14 @@
       </c>
       <c r="N50" s="13"/>
       <c r="O50" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P50" s="21"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="34"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -2680,42 +2973,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32"/>
+      <c r="B54" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="34"/>
+      <c r="N54" s="34"/>
+      <c r="O54" s="34"/>
+      <c r="P54" s="34"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
+      <c r="B55" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="34"/>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34"/>
+      <c r="M55" s="34"/>
+      <c r="N55" s="34"/>
+      <c r="O55" s="34"/>
+      <c r="P55" s="34"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -2768,4 +3061,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Data for Night 4 & 5
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Hier die Ergebnisse der bis zu 10 Matchboxen eintragen. Spalte KandidatInA&amp;B sowie Match sind Pflicht, Unique optional für Auswertung (nur bei Match relevant)</t>
+  </si>
+  <si>
+    <t>Box 6, Folge 10 - 11</t>
+  </si>
+  <si>
+    <t>Box 6, doppeltes Match zu Caroline</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,6 +533,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -535,9 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,11 +560,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -577,6 +586,69 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1104,12 +1176,12 @@
       <c r="F13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E15" s="7" t="s">
@@ -1120,26 +1192,26 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="20" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -1164,17 +1236,17 @@
     <mergeCell ref="B18:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F13">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C12">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1213,16 +1285,16 @@
   <sheetData>
     <row r="1" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="AD2" s="8" t="s">
         <v>10</v>
       </c>
@@ -1341,9 +1413,15 @@
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F8" s="30"/>
       <c r="G8" s="10"/>
       <c r="H8" s="30"/>
@@ -1355,25 +1433,45 @@
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="30"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" s="30"/>
-      <c r="I9" s="7"/>
+      <c r="I9" s="28" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F10" s="30"/>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" s="30"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
@@ -1427,9 +1525,9 @@
       <c r="B15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="30"/>
       <c r="G15" s="10"/>
       <c r="H15" s="30"/>
@@ -1439,148 +1537,148 @@
       <c r="B16" s="9">
         <v>13</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="30"/>
       <c r="G16" s="10"/>
       <c r="H16" s="30"/>
-      <c r="I16" s="7"/>
+      <c r="I16" s="28"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>14</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="30"/>
       <c r="G17" s="10"/>
       <c r="H17" s="30"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="28"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>15</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="31"/>
       <c r="F18" s="30"/>
       <c r="G18" s="10"/>
       <c r="H18" s="30"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>16</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="30"/>
       <c r="G19" s="10"/>
       <c r="H19" s="30"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>17</v>
       </c>
-      <c r="C20" s="10"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="31"/>
       <c r="F20" s="30"/>
       <c r="G20" s="10"/>
       <c r="H20" s="30"/>
-      <c r="I20" s="7"/>
+      <c r="I20" s="28"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>18</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="30"/>
       <c r="G21" s="10"/>
       <c r="H21" s="30"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>19</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="30"/>
       <c r="G22" s="10"/>
       <c r="H22" s="30"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="28"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>20</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="31"/>
       <c r="F23" s="30"/>
       <c r="G23" s="10"/>
       <c r="H23" s="30"/>
-      <c r="I23" s="7"/>
+      <c r="I23" s="28"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -1593,22 +1691,67 @@
     <mergeCell ref="B26:N26"/>
     <mergeCell ref="B27:N27"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:H7 C9:H10 C12:H23">
+  <conditionalFormatting sqref="C4:H7 C9:H10 C12:H14 C15:D23 F15:H23">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:H8">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:H11">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:H8">
+  <conditionalFormatting sqref="E22">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:H11">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G23 E4:E23">
       <formula1>$AD$3:$AD$4</formula1>
     </dataValidation>
@@ -1616,7 +1759,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>TeilnehmerInnen!$F$3:$F$13</xm:f>
@@ -1640,7 +1783,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,18 +2344,40 @@
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
       <c r="C21" s="36"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="D21" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>34</v>
+      </c>
       <c r="N21" s="13"/>
-      <c r="O21" s="27"/>
+      <c r="O21" s="27">
+        <v>3</v>
+      </c>
       <c r="P21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2973,42 +3138,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="34"/>
-      <c r="N55" s="34"/>
-      <c r="O55" s="34"/>
-      <c r="P55" s="34"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3016,6 +3181,12 @@
     <protectedRange sqref="D6:O6 D11:O11 D16:O16 D21:O21 D26:O26 D31:O31 D36:O36 D41:O41 D46:O46 D51:O51" name="Bereich1"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C25:C26"/>
@@ -3023,12 +3194,6 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 1 & 2
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -138,100 +138,76 @@
     <t>Falls NachzüglerIn als zusätzliches Match bekannt ist, unbedingt bei ID 11 eintragen und Kästchen auf "ja" setzen</t>
   </si>
   <si>
-    <t>Barkin</t>
-  </si>
-  <si>
-    <t>Burim</t>
-  </si>
-  <si>
-    <t>Christopher</t>
-  </si>
-  <si>
-    <t>Deniz</t>
-  </si>
-  <si>
-    <t>Joel</t>
-  </si>
-  <si>
-    <t>Ken</t>
-  </si>
-  <si>
-    <t>Kenneth</t>
-  </si>
-  <si>
-    <t>Maximilian</t>
-  </si>
-  <si>
-    <t>Pascal</t>
-  </si>
-  <si>
-    <t>Sasa</t>
-  </si>
-  <si>
-    <t>Marwin</t>
-  </si>
-  <si>
-    <t>Aurelia</t>
-  </si>
-  <si>
-    <t>Carina</t>
-  </si>
-  <si>
-    <t>Caroline</t>
-  </si>
-  <si>
-    <t>Dorna</t>
-  </si>
-  <si>
-    <t>Henna</t>
-  </si>
-  <si>
-    <t>Juliette</t>
-  </si>
-  <si>
-    <t>Larissa</t>
-  </si>
-  <si>
     <t>Stefanie</t>
   </si>
   <si>
-    <t>Vanessa</t>
-  </si>
-  <si>
-    <t>Valeria</t>
-  </si>
-  <si>
-    <t>Box 1, Folge 1</t>
-  </si>
-  <si>
-    <t>Box 5, Folge 8 - 9</t>
-  </si>
-  <si>
-    <t>Box 4, Folge 6 - 7</t>
-  </si>
-  <si>
-    <t>Box 3, Folge 4 - 5</t>
-  </si>
-  <si>
-    <t>Box 2, Folge 2 - 3</t>
-  </si>
-  <si>
     <t>Hier die Ergebnisse der bis zu 10 Matchboxen eintragen. Spalte KandidatInA&amp;B sowie Match sind Pflicht, Unique optional für Auswertung (nur bei Match relevant)</t>
   </si>
   <si>
-    <t>Box 6, Folge 10 - 11</t>
-  </si>
-  <si>
-    <t>Box 6, doppeltes Match zu Caroline</t>
-  </si>
-  <si>
-    <t>Box 7, Folge 12 - 13</t>
-  </si>
-  <si>
-    <t>Box 8, Folge 14-15</t>
-  </si>
-  <si>
-    <t>Box 9, Folge 16-17</t>
+    <t>Alicia</t>
+  </si>
+  <si>
+    <t>Christina</t>
+  </si>
+  <si>
+    <t>Danilo</t>
+  </si>
+  <si>
+    <t>Darya</t>
+  </si>
+  <si>
+    <t>Elia</t>
+  </si>
+  <si>
+    <t>Emanuell</t>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Jenny</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Paco</t>
+  </si>
+  <si>
+    <t>Paulina</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Sabrina</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Steffen</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 2</t>
+  </si>
+  <si>
+    <t>M. Teezy</t>
+  </si>
+  <si>
+    <t>Kim V.</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 4</t>
   </si>
 </sst>
 </file>
@@ -1009,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,13 +1019,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -1057,13 +1033,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -1071,13 +1047,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -1085,13 +1061,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -1099,13 +1075,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -1113,13 +1089,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -1127,13 +1103,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -1141,13 +1117,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -1155,13 +1131,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1169,13 +1145,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -1183,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>4</v>
@@ -1194,7 +1170,7 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E15" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>23</v>
@@ -1274,7 +1250,7 @@
   <dimension ref="B1:AD27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>12</v>
@@ -1350,7 +1326,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="30"/>
       <c r="I4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>12</v>
@@ -1361,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>31</v>
@@ -1373,174 +1349,104 @@
       <c r="G5" s="10"/>
       <c r="H5" s="30"/>
       <c r="I5" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="G7" s="10"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="30"/>
       <c r="G8" s="10"/>
       <c r="H8" s="30"/>
-      <c r="I8" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="30"/>
-      <c r="G9" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="G9" s="10"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="28" t="s">
-        <v>52</v>
-      </c>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="G10" s="10"/>
       <c r="H10" s="30"/>
-      <c r="I10" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="30"/>
       <c r="G11" s="10"/>
       <c r="H11" s="30"/>
-      <c r="I11" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="30"/>
       <c r="G12" s="10"/>
       <c r="H12" s="30"/>
-      <c r="I12" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="30"/>
       <c r="G13" s="10"/>
       <c r="H13" s="30"/>
-      <c r="I13" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
@@ -1664,7 +1570,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="32" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C25" s="32"/>
       <c r="D25" s="32"/>
@@ -1815,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,43 +1800,43 @@
       </c>
       <c r="D5" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F5" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G5" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H5" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I5" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J5" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K5" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L5" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M5" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="26" t="s">
@@ -1943,34 +1849,34 @@
       <c r="B6" s="16"/>
       <c r="C6" s="37"/>
       <c r="D6" s="7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="27">
@@ -2039,43 +1945,43 @@
       </c>
       <c r="D10" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E10" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F10" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G10" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H10" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I10" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J10" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K10" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L10" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M10" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="26" t="s">
@@ -2088,38 +1994,38 @@
       <c r="B11" s="16"/>
       <c r="C11" s="37"/>
       <c r="D11" s="7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>29</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P11" s="21"/>
     </row>
@@ -2184,43 +2090,43 @@
       </c>
       <c r="D15" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E15" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F15" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G15" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H15" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I15" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J15" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K15" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L15" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M15" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="26" t="s">
@@ -2232,40 +2138,18 @@
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
       <c r="C16" s="37"/>
-      <c r="D16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="13"/>
-      <c r="O16" s="27">
-        <v>2</v>
-      </c>
+      <c r="O16" s="27"/>
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2329,43 +2213,43 @@
       </c>
       <c r="D20" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E20" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F20" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G20" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H20" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I20" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J20" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K20" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L20" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M20" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N20" s="13"/>
       <c r="O20" s="26" t="s">
@@ -2377,40 +2261,18 @@
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
       <c r="C21" s="37"/>
-      <c r="D21" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21" s="28" t="s">
-        <v>34</v>
-      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="27">
-        <v>3</v>
-      </c>
+      <c r="O21" s="27"/>
       <c r="P21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2474,43 +2336,43 @@
       </c>
       <c r="D25" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E25" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F25" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G25" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H25" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I25" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J25" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K25" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L25" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M25" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N25" s="13"/>
       <c r="O25" s="26" t="s">
@@ -2522,40 +2384,18 @@
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
       <c r="C26" s="37"/>
-      <c r="D26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
       <c r="N26" s="13"/>
-      <c r="O26" s="27">
-        <v>4</v>
-      </c>
+      <c r="O26" s="27"/>
       <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2619,43 +2459,43 @@
       </c>
       <c r="D30" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E30" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F30" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G30" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H30" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I30" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J30" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K30" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L30" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M30" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="26" t="s">
@@ -2667,40 +2507,18 @@
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
       <c r="C31" s="37"/>
-      <c r="D31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
       <c r="N31" s="13"/>
-      <c r="O31" s="27">
-        <v>3</v>
-      </c>
+      <c r="O31" s="27"/>
       <c r="P31" s="21"/>
     </row>
     <row r="32" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2764,43 +2582,43 @@
       </c>
       <c r="D35" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E35" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F35" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G35" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H35" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I35" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J35" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K35" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L35" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M35" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="26" t="s">
@@ -2812,40 +2630,18 @@
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
       <c r="C36" s="37"/>
-      <c r="D36" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>28</v>
-      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
       <c r="N36" s="13"/>
-      <c r="O36" s="27">
-        <v>2</v>
-      </c>
+      <c r="O36" s="27"/>
       <c r="P36" s="21"/>
     </row>
     <row r="37" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2909,43 +2705,43 @@
       </c>
       <c r="D40" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E40" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F40" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G40" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H40" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I40" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J40" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K40" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L40" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M40" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N40" s="13"/>
       <c r="O40" s="26" t="s">
@@ -2957,40 +2753,18 @@
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
       <c r="C41" s="37"/>
-      <c r="D41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
       <c r="N41" s="13"/>
-      <c r="O41" s="27">
-        <v>2</v>
-      </c>
+      <c r="O41" s="27"/>
       <c r="P41" s="21"/>
     </row>
     <row r="42" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3054,43 +2828,43 @@
       </c>
       <c r="D45" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E45" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F45" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G45" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H45" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I45" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J45" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K45" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L45" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M45" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N45" s="13"/>
       <c r="O45" s="26" t="s">
@@ -3177,43 +2951,43 @@
       </c>
       <c r="D50" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Aurelia</v>
+        <v>Alicia</v>
       </c>
       <c r="E50" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Carina</v>
+        <v>Christina</v>
       </c>
       <c r="F50" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Caroline</v>
+        <v>Darya</v>
       </c>
       <c r="G50" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Dorna</v>
+        <v>Jenny</v>
       </c>
       <c r="H50" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Henna</v>
+        <v>Kim V.</v>
       </c>
       <c r="I50" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Juliette</v>
+        <v>Marie</v>
       </c>
       <c r="J50" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Larissa</v>
+        <v>Paulina</v>
       </c>
       <c r="K50" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Stefanie</v>
+        <v>Sabrina</v>
       </c>
       <c r="L50" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Valeria</v>
+        <v>Sandra</v>
       </c>
       <c r="M50" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Vanessa</v>
+        <v>Stefanie</v>
       </c>
       <c r="N50" s="13"/>
       <c r="O50" s="26" t="s">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 3
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Matchbox Folge 4</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 6</t>
   </si>
 </sst>
 </file>
@@ -530,9 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -547,6 +547,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -985,7 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1250,7 +1253,7 @@
   <dimension ref="B1:AD27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,13 +1359,21 @@
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
@@ -1721,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,23 +1750,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="40"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1795,7 +1806,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
@@ -1847,7 +1858,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1940,7 +1951,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
@@ -1992,7 +2003,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="37"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2085,7 +2096,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="36">
+      <c r="C15" s="35">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
@@ -2137,19 +2148,41 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="N16" s="13"/>
-      <c r="O16" s="27"/>
+      <c r="O16" s="27">
+        <v>2</v>
+      </c>
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2208,7 +2241,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="36">
+      <c r="C20" s="35">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
@@ -2260,7 +2293,7 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
@@ -2331,7 +2364,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="36">
+      <c r="C25" s="35">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
@@ -2383,7 +2416,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="37"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2454,7 +2487,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="36">
+      <c r="C30" s="35">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
@@ -2506,7 +2539,7 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="37"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2577,7 +2610,7 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="36">
+      <c r="C35" s="35">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
@@ -2629,7 +2662,7 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="37"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2700,7 +2733,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="36">
+      <c r="C40" s="35">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
@@ -2752,7 +2785,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="37"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2823,7 +2856,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="36">
+      <c r="C45" s="35">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -2875,7 +2908,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="37"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2946,7 +2979,7 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="36">
+      <c r="C50" s="35">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
@@ -2998,7 +3031,7 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="37"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3033,42 +3066,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
-      <c r="N54" s="35"/>
-      <c r="O54" s="35"/>
-      <c r="P54" s="35"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="35"/>
-      <c r="P55" s="35"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3076,6 +3109,12 @@
     <protectedRange sqref="D6:O6 D11:O11 D16:O16 D21:O21 D26:O26 D31:O31 D36:O36 D41:O41 D46:O46 D51:O51" name="Bereich1"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C25:C26"/>
@@ -3083,12 +3122,6 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 4
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -198,19 +198,22 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Matchbox Folge 2</t>
-  </si>
-  <si>
     <t>M. Teezy</t>
   </si>
   <si>
     <t>Kim V.</t>
   </si>
   <si>
-    <t>Matchbox Folge 4</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 6</t>
+    <t>Matchbox Folge 6 (+7)</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 4 (+5)</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 2 (+3)</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 8 (+9)</t>
   </si>
 </sst>
 </file>
@@ -533,6 +536,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -547,9 +553,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,13 +1081,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -1253,7 +1256,7 @@
   <dimension ref="B1:AD27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1332,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="30"/>
       <c r="I4" s="7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>12</v>
@@ -1372,20 +1375,28 @@
       <c r="G6" s="10"/>
       <c r="H6" s="30"/>
       <c r="I6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F7" s="30"/>
       <c r="G7" s="10"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
@@ -1732,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,23 +1761,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1806,7 +1817,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="35">
+      <c r="C5" s="36">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
@@ -1858,7 +1869,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1887,7 +1898,7 @@
         <v>38</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="27">
@@ -1951,7 +1962,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="35">
+      <c r="C10" s="36">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
@@ -2003,7 +2014,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="36"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2032,7 +2043,7 @@
         <v>31</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="27">
@@ -2096,7 +2107,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="35">
+      <c r="C15" s="36">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
@@ -2148,7 +2159,7 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
@@ -2162,7 +2173,7 @@
         <v>32</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>31</v>
@@ -2241,7 +2252,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
@@ -2293,19 +2304,41 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="N21" s="13"/>
-      <c r="O21" s="27"/>
+      <c r="O21" s="27">
+        <v>4</v>
+      </c>
       <c r="P21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2364,7 +2397,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="35">
+      <c r="C25" s="36">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
@@ -2416,7 +2449,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2487,7 +2520,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="35">
+      <c r="C30" s="36">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
@@ -2539,7 +2572,7 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -2610,7 +2643,7 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="35">
+      <c r="C35" s="36">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
@@ -2662,7 +2695,7 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="36"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2733,7 +2766,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="35">
+      <c r="C40" s="36">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
@@ -2785,7 +2818,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="36"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2856,7 +2889,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="35">
+      <c r="C45" s="36">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -2908,7 +2941,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2979,7 +3012,7 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="35">
+      <c r="C50" s="36">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
@@ -3031,7 +3064,7 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="36"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3066,42 +3099,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="40"/>
-      <c r="P54" s="40"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="35"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="40"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
-      <c r="P55" s="40"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="35"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3109,12 +3142,6 @@
     <protectedRange sqref="D6:O6 D11:O11 D16:O16 D21:O21 D26:O26 D31:O31 D36:O36 D41:O41 D46:O46 D51:O51" name="Bereich1"/>
   </protectedRanges>
   <mergeCells count="13">
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C25:C26"/>
@@ -3122,6 +3149,12 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 5
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Matchbox Folge 8 (+9)</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 10 (+11)</t>
   </si>
 </sst>
 </file>
@@ -991,7 +994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1255,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,20 +1405,34 @@
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="30"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="30"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="30"/>
       <c r="G9" s="10"/>
@@ -1744,7 +1761,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,18 +2467,40 @@
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
       <c r="C26" s="37"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="N26" s="13"/>
-      <c r="O26" s="27"/>
+      <c r="O26" s="27">
+        <v>4</v>
+      </c>
       <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 6 + Fix Nacht 5
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Matchbox Folge 10 (+11)</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 12 (+13)</t>
   </si>
 </sst>
 </file>
@@ -539,9 +542,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,6 +556,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,11 +1436,15 @@
       <c r="D9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="F9" s="30"/>
       <c r="G9" s="10"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="28"/>
+      <c r="I9" s="28" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
@@ -1760,7 +1767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -1778,23 +1785,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="40"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1834,7 +1841,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
@@ -1886,7 +1893,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1979,7 +1986,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
@@ -2031,7 +2038,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="37"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2124,7 +2131,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="36">
+      <c r="C15" s="35">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
@@ -2176,7 +2183,7 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="37"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
@@ -2269,7 +2276,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="36">
+      <c r="C20" s="35">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
@@ -2321,7 +2328,7 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="37"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="28" t="s">
         <v>45</v>
       </c>
@@ -2414,7 +2421,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="36">
+      <c r="C25" s="35">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
@@ -2466,7 +2473,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="37"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="7" t="s">
         <v>43</v>
       </c>
@@ -2499,7 +2506,7 @@
       </c>
       <c r="N26" s="13"/>
       <c r="O26" s="27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P26" s="21"/>
     </row>
@@ -2559,7 +2566,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="36">
+      <c r="C30" s="35">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
@@ -2611,19 +2618,41 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="N31" s="13"/>
-      <c r="O31" s="27"/>
+      <c r="O31" s="27">
+        <v>4</v>
+      </c>
       <c r="P31" s="21"/>
     </row>
     <row r="32" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2682,7 +2711,7 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="36">
+      <c r="C35" s="35">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
@@ -2734,7 +2763,7 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="37"/>
+      <c r="C36" s="36"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2805,7 +2834,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="36">
+      <c r="C40" s="35">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
@@ -2857,7 +2886,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="37"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2928,7 +2957,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="36">
+      <c r="C45" s="35">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -2980,7 +3009,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="37"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -3051,7 +3080,7 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="36">
+      <c r="C50" s="35">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
@@ -3103,7 +3132,7 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="37"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3138,42 +3167,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
-      <c r="N54" s="35"/>
-      <c r="O54" s="35"/>
-      <c r="P54" s="35"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="40"/>
+      <c r="M54" s="40"/>
+      <c r="N54" s="40"/>
+      <c r="O54" s="40"/>
+      <c r="P54" s="40"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="35"/>
-      <c r="P55" s="35"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="40"/>
+      <c r="J55" s="40"/>
+      <c r="K55" s="40"/>
+      <c r="L55" s="40"/>
+      <c r="M55" s="40"/>
+      <c r="N55" s="40"/>
+      <c r="O55" s="40"/>
+      <c r="P55" s="40"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3181,6 +3210,12 @@
     <protectedRange sqref="D6:O6 D11:O11 D16:O16 D21:O21 D26:O26 D31:O31 D36:O36 D41:O41 D46:O46 D51:O51" name="Bereich1"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C25:C26"/>
@@ -3188,12 +3223,6 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 7
Implementierung für bekanntes Doppelmatch hart gecoded => TODO => muss noch gefixt werden
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Matchbox Folge 12 (+13)</t>
+  </si>
+  <si>
+    <t>Folge 14/15: Max/Peter sind doppeltes Match</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1265,7 @@
   <dimension ref="B1:AD27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B25" sqref="B25:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1459,9 @@
       <c r="F10" s="30"/>
       <c r="G10" s="10"/>
       <c r="H10" s="30"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
@@ -1768,7 +1773,7 @@
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,18 +2769,40 @@
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
       <c r="C36" s="36"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
+      <c r="D36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="N36" s="13"/>
-      <c r="O36" s="27"/>
+      <c r="O36" s="27">
+        <v>3</v>
+      </c>
       <c r="P36" s="21"/>
     </row>
     <row r="37" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update AYTO VIP 2023 Nacht 8
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Folge 14/15: Max/Peter sind doppeltes Match</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 16 (+17)</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,21 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1236,17 +1253,17 @@
     <mergeCell ref="B18:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F13">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C12">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1264,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,14 +1470,20 @@
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>12</v>
+      </c>
       <c r="F10" s="30"/>
       <c r="G10" s="10"/>
       <c r="H10" s="30"/>
-      <c r="I10" s="7" t="s">
-        <v>53</v>
+      <c r="I10" s="28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
@@ -1473,7 +1496,9 @@
       <c r="F11" s="30"/>
       <c r="G11" s="10"/>
       <c r="H11" s="30"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="28" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
@@ -1681,63 +1706,68 @@
     <mergeCell ref="B26:N26"/>
     <mergeCell ref="B27:N27"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:H7 C9:H10 C12:H14 C15:D23 F15:H23">
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="notEqual">
+  <conditionalFormatting sqref="C4:H7 C9:H9 C12:H14 C15:D23 F15:H23 F10:H10">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:H8">
-    <cfRule type="cellIs" dxfId="14" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:H11">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:E10">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1772,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2914,18 +2944,40 @@
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
       <c r="C41" s="36"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
+      <c r="D41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="N41" s="13"/>
-      <c r="O41" s="27"/>
+      <c r="O41" s="27">
+        <v>1</v>
+      </c>
       <c r="P41" s="21"/>
     </row>
     <row r="42" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3252,19 +3304,19 @@
     <mergeCell ref="C5:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6 O11 O16 O21 O26 O31 O36 O41 O46 O51">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>0</formula>
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hinzufügen Kurzerklärung zum Skript
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -548,6 +548,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,28 +566,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -603,6 +589,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1253,17 +1246,17 @@
     <mergeCell ref="B18:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F13">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C12">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1282,7 +1275,7 @@
   <dimension ref="B1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C11" sqref="C11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,67 +1700,67 @@
     <mergeCell ref="B27:N27"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:H7 C9:H9 C12:H14 C15:D23 F15:H23 F10:H10">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:H8">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:H11">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:E10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1820,23 +1813,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1876,7 +1869,7 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="35">
+      <c r="C5" s="36">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
@@ -1928,7 +1921,7 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="36"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
@@ -2021,7 +2014,7 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="35">
+      <c r="C10" s="36">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
@@ -2073,7 +2066,7 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="36"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="7" t="s">
         <v>43</v>
       </c>
@@ -2166,7 +2159,7 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="35">
+      <c r="C15" s="36">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
@@ -2218,7 +2211,7 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
@@ -2311,7 +2304,7 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
@@ -2363,7 +2356,7 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="28" t="s">
         <v>45</v>
       </c>
@@ -2456,7 +2449,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="35">
+      <c r="C25" s="36">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
@@ -2508,7 +2501,7 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="7" t="s">
         <v>43</v>
       </c>
@@ -2601,7 +2594,7 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="35">
+      <c r="C30" s="36">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
@@ -2653,7 +2646,7 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="36"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="7" t="s">
         <v>38</v>
       </c>
@@ -2746,7 +2739,7 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="35">
+      <c r="C35" s="36">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
@@ -2798,7 +2791,7 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="36"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="7" t="s">
         <v>33</v>
       </c>
@@ -2891,7 +2884,7 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="35">
+      <c r="C40" s="36">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
@@ -2943,7 +2936,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="36"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="7" t="s">
         <v>40</v>
       </c>
@@ -3036,7 +3029,7 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="35">
+      <c r="C45" s="36">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
@@ -3088,7 +3081,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="36"/>
+      <c r="C46" s="37"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -3159,7 +3152,7 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="35">
+      <c r="C50" s="36">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
@@ -3211,7 +3204,7 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="36"/>
+      <c r="C51" s="37"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3246,42 +3239,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="40"/>
-      <c r="P54" s="40"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="35"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="40"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="40"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
-      <c r="P55" s="40"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="35"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3289,12 +3282,6 @@
     <protectedRange sqref="D6:O6 D11:O11 D16:O16 D21:O21 D26:O26 D31:O31 D36:O36 D41:O41 D46:O46 D51:O51" name="Bereich1"/>
   </protectedRanges>
   <mergeCells count="13">
-    <mergeCell ref="B54:P54"/>
-    <mergeCell ref="B55:P55"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C35:C36"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C25:C26"/>
@@ -3302,21 +3289,27 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B54:P54"/>
+    <mergeCell ref="B55:P55"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C35:C36"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6 O11 O16 O21 O26 O31 O36 O41 O46 O51">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
AYTO VIP 2024 Nacht1
</commit_message>
<xml_diff>
--- a/AYTO_Berechnung/AYTO_Data.xlsx
+++ b/AYTO_Berechnung/AYTO_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TeilnehmerInnen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -135,96 +135,9 @@
     <t>Falls NachzüglerIn als zusätzliches Match bekannt ist, unbedingt bei ID 11 eintragen und Kästchen auf "ja" setzen</t>
   </si>
   <si>
-    <t>Stefanie</t>
-  </si>
-  <si>
     <t>Hier die Ergebnisse der bis zu 10 Matchboxen eintragen. Spalte KandidatInA&amp;B sowie Match sind Pflicht, Unique optional für Auswertung (nur bei Match relevant)</t>
   </si>
   <si>
-    <t>Alicia</t>
-  </si>
-  <si>
-    <t>Christina</t>
-  </si>
-  <si>
-    <t>Danilo</t>
-  </si>
-  <si>
-    <t>Darya</t>
-  </si>
-  <si>
-    <t>Elia</t>
-  </si>
-  <si>
-    <t>Emanuell</t>
-  </si>
-  <si>
-    <t>Fabio</t>
-  </si>
-  <si>
-    <t>Jenny</t>
-  </si>
-  <si>
-    <t>Marie</t>
-  </si>
-  <si>
-    <t>Marvin</t>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Paco</t>
-  </si>
-  <si>
-    <t>Paulina</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>Sandra</t>
-  </si>
-  <si>
-    <t>Steffen</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>M. Teezy</t>
-  </si>
-  <si>
-    <t>Kim V.</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 6 (+7)</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 4 (+5)</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 2 (+3)</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 8 (+9)</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 10 (+11)</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 12 (+13)</t>
-  </si>
-  <si>
-    <t>Folge 14/15: Max/Peter sind doppeltes Match</t>
-  </si>
-  <si>
-    <t>Matchbox Folge 16 (+17)</t>
-  </si>
-  <si>
     <t>Matchbox doppeltes Match</t>
   </si>
   <si>
@@ -238,6 +151,72 @@
   </si>
   <si>
     <t>Falls ein Doppelmatch gefunden wird, muss Unique auf nein gesetzt werden (alle weiteren NoMatches können manuell ergänzt werden, müssen aber nicht)</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Anastasia</t>
+  </si>
+  <si>
+    <t>Antonino</t>
+  </si>
+  <si>
+    <t>Asena</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Dana</t>
+  </si>
+  <si>
+    <t>Emmy</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Kaan</t>
+  </si>
+  <si>
+    <t>Lars</t>
+  </si>
+  <si>
+    <t>Laura L.</t>
+  </si>
+  <si>
+    <t>Laura M.</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Marc-Robin</t>
+  </si>
+  <si>
+    <t>Nadja</t>
+  </si>
+  <si>
+    <t>Nikola</t>
+  </si>
+  <si>
+    <t>Ozan</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Tara</t>
+  </si>
+  <si>
+    <t>Matchbox Folge 2/3</t>
   </si>
 </sst>
 </file>
@@ -600,6 +579,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -617,37 +614,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -666,6 +638,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -997,7 +976,7 @@
   <dimension ref="B1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,13 +1009,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -1044,13 +1023,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -1058,13 +1037,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -1072,13 +1051,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -1086,13 +1065,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -1100,13 +1079,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -1114,13 +1093,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -1128,13 +1107,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -1142,13 +1121,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1156,13 +1135,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -1170,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G13" s="34" t="s">
         <v>4</v>
@@ -1260,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="C26:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,10 +1304,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>12</v>
@@ -1337,7 +1316,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="30"/>
       <c r="I4" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>12</v>
@@ -1347,123 +1326,73 @@
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="30"/>
       <c r="G5" s="10"/>
       <c r="H5" s="30"/>
-      <c r="I5" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="30"/>
       <c r="G7" s="10"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="30"/>
-      <c r="G8" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="G8" s="10"/>
       <c r="H8" s="30"/>
-      <c r="I8" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>12</v>
-      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="30"/>
       <c r="G9" s="10"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="28" t="s">
-        <v>51</v>
-      </c>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>12</v>
-      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="30"/>
       <c r="G10" s="10"/>
       <c r="H10" s="30"/>
-      <c r="I10" s="28" t="s">
-        <v>53</v>
-      </c>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
@@ -1475,9 +1404,7 @@
       <c r="F11" s="30"/>
       <c r="G11" s="10"/>
       <c r="H11" s="30"/>
-      <c r="I11" s="28" t="s">
-        <v>52</v>
-      </c>
+      <c r="I11" s="28"/>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
@@ -1624,36 +1551,32 @@
       <c r="I23" s="28"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="44"/>
+      <c r="B25" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
-      <c r="C26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="47"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -1687,7 +1610,7 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="33" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -1704,7 +1627,7 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="33" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
@@ -1721,7 +1644,7 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="33" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
@@ -1753,7 +1676,7 @@
     <mergeCell ref="E26:I26"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E23 G4:G23 C26:D26">
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1788,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,23 +1729,23 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="40"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="46"/>
     </row>
     <row r="3" spans="1:16" s="23" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
@@ -1862,48 +1785,48 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="36">
+      <c r="C5" s="42">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E5" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F5" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G5" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H5" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I5" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J5" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K5" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L5" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M5" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="26" t="s">
@@ -1914,40 +1837,40 @@
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="37"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" s="21"/>
     </row>
@@ -2007,48 +1930,48 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="36">
+      <c r="C10" s="42">
         <v>2</v>
       </c>
       <c r="D10" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E10" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F10" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G10" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H10" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I10" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J10" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K10" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L10" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M10" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="26" t="s">
@@ -2059,41 +1982,19 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="13"/>
-      <c r="O11" s="27">
-        <v>2</v>
-      </c>
+      <c r="O11" s="27"/>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2152,48 +2053,48 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="36">
+      <c r="C15" s="42">
         <v>3</v>
       </c>
       <c r="D15" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E15" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F15" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G15" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H15" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I15" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J15" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K15" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L15" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M15" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="26" t="s">
@@ -2204,41 +2105,19 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="13"/>
-      <c r="O16" s="27">
-        <v>2</v>
-      </c>
+      <c r="O16" s="27"/>
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2297,48 +2176,48 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="36">
+      <c r="C20" s="42">
         <v>4</v>
       </c>
       <c r="D20" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E20" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F20" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G20" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H20" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I20" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J20" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K20" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L20" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M20" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N20" s="13"/>
       <c r="O20" s="26" t="s">
@@ -2349,41 +2228,19 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="L21" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="M21" s="28" t="s">
-        <v>31</v>
-      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="27">
-        <v>4</v>
-      </c>
+      <c r="O21" s="27"/>
       <c r="P21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2442,48 +2299,48 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="36">
+      <c r="C25" s="42">
         <v>5</v>
       </c>
       <c r="D25" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E25" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F25" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G25" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H25" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I25" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J25" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K25" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L25" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M25" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N25" s="13"/>
       <c r="O25" s="26" t="s">
@@ -2494,41 +2351,19 @@
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M26" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
       <c r="N26" s="13"/>
-      <c r="O26" s="27">
-        <v>3</v>
-      </c>
+      <c r="O26" s="27"/>
       <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2587,48 +2422,48 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="36">
+      <c r="C30" s="42">
         <v>6</v>
       </c>
       <c r="D30" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E30" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F30" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G30" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H30" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I30" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J30" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K30" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L30" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M30" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N30" s="13"/>
       <c r="O30" s="26" t="s">
@@ -2639,41 +2474,19 @@
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M31" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
       <c r="N31" s="13"/>
-      <c r="O31" s="27">
-        <v>4</v>
-      </c>
+      <c r="O31" s="27"/>
       <c r="P31" s="21"/>
     </row>
     <row r="32" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2732,48 +2545,48 @@
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="36">
+      <c r="C35" s="42">
         <v>7</v>
       </c>
       <c r="D35" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E35" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F35" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G35" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H35" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I35" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J35" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K35" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L35" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M35" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N35" s="13"/>
       <c r="O35" s="26" t="s">
@@ -2784,41 +2597,19 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="C36" s="43"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
       <c r="N36" s="13"/>
-      <c r="O36" s="27">
-        <v>3</v>
-      </c>
+      <c r="O36" s="27"/>
       <c r="P36" s="21"/>
     </row>
     <row r="37" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2877,48 +2668,48 @@
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="36">
+      <c r="C40" s="42">
         <v>8</v>
       </c>
       <c r="D40" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E40" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F40" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G40" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H40" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I40" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J40" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K40" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L40" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M40" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N40" s="13"/>
       <c r="O40" s="26" t="s">
@@ -2929,41 +2720,19 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="C41" s="43"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
       <c r="N41" s="13"/>
-      <c r="O41" s="27">
-        <v>1</v>
-      </c>
+      <c r="O41" s="27"/>
       <c r="P41" s="21"/>
     </row>
     <row r="42" spans="1:16" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3022,48 +2791,48 @@
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="36">
+      <c r="C45" s="42">
         <v>9</v>
       </c>
       <c r="D45" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E45" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F45" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G45" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H45" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I45" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J45" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K45" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L45" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M45" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N45" s="13"/>
       <c r="O45" s="26" t="s">
@@ -3074,7 +2843,7 @@
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="37"/>
+      <c r="C46" s="43"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -3145,48 +2914,48 @@
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="36">
+      <c r="C50" s="42">
         <v>10</v>
       </c>
       <c r="D50" s="12" t="str">
         <f>TeilnehmerInnen!$C$3</f>
-        <v>Alicia</v>
+        <v>Alex</v>
       </c>
       <c r="E50" s="12" t="str">
         <f>TeilnehmerInnen!$C$4</f>
-        <v>Christina</v>
+        <v>Antonino</v>
       </c>
       <c r="F50" s="12" t="str">
         <f>TeilnehmerInnen!$C$5</f>
-        <v>Darya</v>
+        <v>Chris</v>
       </c>
       <c r="G50" s="12" t="str">
         <f>TeilnehmerInnen!$C$6</f>
-        <v>Jenny</v>
+        <v>Kaan</v>
       </c>
       <c r="H50" s="12" t="str">
         <f>TeilnehmerInnen!$C$7</f>
-        <v>Kim V.</v>
+        <v>Lars</v>
       </c>
       <c r="I50" s="12" t="str">
         <f>TeilnehmerInnen!$C$8</f>
-        <v>Marie</v>
+        <v>Lukas</v>
       </c>
       <c r="J50" s="12" t="str">
         <f>TeilnehmerInnen!$C$9</f>
-        <v>Paulina</v>
+        <v>Marc-Robin</v>
       </c>
       <c r="K50" s="12" t="str">
         <f>TeilnehmerInnen!$C$10</f>
-        <v>Sabrina</v>
+        <v>Nikola</v>
       </c>
       <c r="L50" s="12" t="str">
         <f>TeilnehmerInnen!$C$11</f>
-        <v>Sandra</v>
+        <v>Ozan</v>
       </c>
       <c r="M50" s="12" t="str">
         <f>TeilnehmerInnen!$C$12</f>
-        <v>Stefanie</v>
+        <v>Tim</v>
       </c>
       <c r="N50" s="13"/>
       <c r="O50" s="26" t="s">
@@ -3197,7 +2966,7 @@
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="37"/>
+      <c r="C51" s="43"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3232,42 +3001,42 @@
     </row>
     <row r="53" spans="1:16" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="41"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="41"/>
-      <c r="L54" s="41"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="41"/>
-      <c r="O54" s="41"/>
-      <c r="P54" s="41"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
+      <c r="I54" s="47"/>
+      <c r="J54" s="47"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="47"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
+      <c r="P54" s="47"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="41"/>
-      <c r="L55" s="41"/>
-      <c r="M55" s="41"/>
-      <c r="N55" s="41"/>
-      <c r="O55" s="41"/>
-      <c r="P55" s="41"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
+      <c r="N55" s="47"/>
+      <c r="O55" s="47"/>
+      <c r="P55" s="47"/>
     </row>
   </sheetData>
   <sheetProtection password="CA39" sheet="1" objects="1" scenarios="1"/>
@@ -3290,19 +3059,19 @@
     <mergeCell ref="C5:C6"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:M16 D11:M11 D6:M6 D26:M26 D31:M31 D36:M36 D41:M41 D46:M46 D51:M51 D21:M21">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6 O11 O16 O21 O26 O31 O36 O41 O46 O51">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0</formula>
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>